<commit_message>
ajustado restaurar backup com todos os campos da base
</commit_message>
<xml_diff>
--- a/app/static/board/files/exemplo_backup.xlsx
+++ b/app/static/board/files/exemplo_backup.xlsx
@@ -5,23 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Dashflux\app\static\board\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CBE06A9-F512-487D-BDB2-5203E2C95E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF78E68C-CB98-410F-A89C-510EEB8692E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-9255" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="-9255" windowWidth="19410" windowHeight="15585" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conta_corrente" sheetId="1" r:id="rId1"/>
     <sheet name="cartao_credito" sheetId="2" r:id="rId2"/>
+    <sheet name="estabelecimentos" sheetId="3" r:id="rId3"/>
+    <sheet name="contas" sheetId="4" r:id="rId4"/>
+    <sheet name="categorias" sheetId="5" r:id="rId5"/>
+    <sheet name="cartoes" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>data</t>
   </si>
@@ -44,9 +48,6 @@
     <t>28/02/2024</t>
   </si>
   <si>
-    <t>Conta Padrão</t>
-  </si>
-  <si>
     <t>cartao</t>
   </si>
   <si>
@@ -90,6 +91,42 @@
   </si>
   <si>
     <t>SORVETE</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>bandeira</t>
+  </si>
+  <si>
+    <t>ultimos_4_digitos</t>
+  </si>
+  <si>
+    <t>dia_vencimento</t>
+  </si>
+  <si>
+    <t>OUTRO</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>se_banco</t>
+  </si>
+  <si>
+    <t>se_banco_nome</t>
+  </si>
+  <si>
+    <t>se_banco_agencia</t>
+  </si>
+  <si>
+    <t>se_banco_conta</t>
+  </si>
+  <si>
+    <t>ITAU</t>
   </si>
 </sst>
 </file>
@@ -145,12 +182,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +509,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,16 +542,16 @@
         <v>45383</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
       <c r="E2">
         <v>-1000.58</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -506,16 +559,16 @@
         <v>45384</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
       <c r="E3">
         <v>43.05</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -523,13 +576,13 @@
         <v>45385</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>10.11</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +595,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,10 +626,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -584,22 +637,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -607,19 +660,19 @@
         <v>45379</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3">
         <v>100.04</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -627,22 +680,219 @@
         <v>45319</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>-80</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D403186A-CBDE-4576-8F70-7BFE79DC98D8}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719A3378-1539-41F3-B44C-E5A3204FF815}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C29CFD-F9BD-4B31-9F51-828D1FA49F7D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC9B637-9BEA-4E41-ACBC-C54E6EF401F2}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
85 enh adicionar todas as informações ao extrair o backup (#86)
* backup implementado, extração dos dados ok no xlsx

* ajustado restaurar backup com todos os campos da base
</commit_message>
<xml_diff>
--- a/app/static/board/files/exemplo_backup.xlsx
+++ b/app/static/board/files/exemplo_backup.xlsx
@@ -5,23 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Dashflux\app\static\board\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CBE06A9-F512-487D-BDB2-5203E2C95E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF78E68C-CB98-410F-A89C-510EEB8692E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-9255" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="-9255" windowWidth="19410" windowHeight="15585" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conta_corrente" sheetId="1" r:id="rId1"/>
     <sheet name="cartao_credito" sheetId="2" r:id="rId2"/>
+    <sheet name="estabelecimentos" sheetId="3" r:id="rId3"/>
+    <sheet name="contas" sheetId="4" r:id="rId4"/>
+    <sheet name="categorias" sheetId="5" r:id="rId5"/>
+    <sheet name="cartoes" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>data</t>
   </si>
@@ -44,9 +48,6 @@
     <t>28/02/2024</t>
   </si>
   <si>
-    <t>Conta Padrão</t>
-  </si>
-  <si>
     <t>cartao</t>
   </si>
   <si>
@@ -90,6 +91,42 @@
   </si>
   <si>
     <t>SORVETE</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>bandeira</t>
+  </si>
+  <si>
+    <t>ultimos_4_digitos</t>
+  </si>
+  <si>
+    <t>dia_vencimento</t>
+  </si>
+  <si>
+    <t>OUTRO</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>se_banco</t>
+  </si>
+  <si>
+    <t>se_banco_nome</t>
+  </si>
+  <si>
+    <t>se_banco_agencia</t>
+  </si>
+  <si>
+    <t>se_banco_conta</t>
+  </si>
+  <si>
+    <t>ITAU</t>
   </si>
 </sst>
 </file>
@@ -145,12 +182,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +509,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,16 +542,16 @@
         <v>45383</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
       <c r="E2">
         <v>-1000.58</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -506,16 +559,16 @@
         <v>45384</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
       <c r="E3">
         <v>43.05</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -523,13 +576,13 @@
         <v>45385</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>10.11</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +595,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,10 +626,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -584,22 +637,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -607,19 +660,19 @@
         <v>45379</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3">
         <v>100.04</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -627,22 +680,219 @@
         <v>45319</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>-80</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D403186A-CBDE-4576-8F70-7BFE79DC98D8}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719A3378-1539-41F3-B44C-E5A3204FF815}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C29CFD-F9BD-4B31-9F51-828D1FA49F7D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC9B637-9BEA-4E41-ACBC-C54E6EF401F2}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>